<commit_message>
created api login crc,boolean,keyword pos neg test cases, executed symlex high speed server
</commit_message>
<xml_diff>
--- a/api/app_api/backlog/login/osName_negative.xlsx
+++ b/api/app_api/backlog/login/osName_negative.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\office\SymlexVPNTestCases\api\app_api\backlog\login\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2387C5F-DD48-4D3F-8CDA-18B5263AD752}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C62DEBF4-AA33-41C6-93E2-5CCB8ED1AA14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -407,7 +407,7 @@
     <t>post request should fail with status code 400</t>
   </si>
   <si>
-    <t>Test Scenario: Login(api) - osName (positive)</t>
+    <t>Test Scenario: Login(api) - osName (negative)</t>
   </si>
 </sst>
 </file>
@@ -1836,7 +1836,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
+      <selection pane="bottomLeft" sqref="A1:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>